<commit_message>
Sun Nov 14 00:37:34 CST 2021
</commit_message>
<xml_diff>
--- a/计划/2021学习计划.xlsx
+++ b/计划/2021学习计划.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16780"/>
+    <workbookView windowWidth="28800" windowHeight="13180"/>
   </bookViews>
   <sheets>
     <sheet name="10" sheetId="1" r:id="rId1"/>
+    <sheet name="11" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
   <si>
     <t>早餐</t>
   </si>
@@ -179,7 +180,17 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
     </r>
   </si>
   <si>
@@ -212,7 +223,17 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>10基础知识</t>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基础知识</t>
     </r>
     <r>
       <rPr>
@@ -232,27 +253,279 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10基础知识</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -317,7 +590,28 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+作业
+作业</t>
     </r>
   </si>
   <si>
@@ -338,7 +632,17 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>20书</t>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
     </r>
     <r>
       <rPr>
@@ -359,21 +663,57 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+作业
+作业</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10基础知识
 </t>
     </r>
@@ -385,16 +725,78 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>20书</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-10基础知识
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10基础知识
 </t>
     </r>
     <r>
@@ -411,43 +813,13 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
 1音频
 作业
 作业</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10基础知识
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
     </r>
   </si>
   <si>
@@ -509,18 +881,385 @@
   <si>
     <t>腿</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+20书
+10基础知识
+20书
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+20书
+10基础知识
+20书
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10基础知识
+20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频
+作业
+作业</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,6 +1276,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,18 +1296,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -568,9 +1351,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -592,7 +1374,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -606,8 +1396,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -622,16 +1426,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -644,54 +1440,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体-简"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -705,18 +1463,11 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体-简"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -725,25 +1476,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.75"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.25"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.5"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -755,103 +1536,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -869,67 +1674,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -977,7 +1734,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -997,6 +1754,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1008,15 +1776,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1038,11 +1797,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1050,8 +1807,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1060,178 +1817,205 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1554,8 +2338,8 @@
   <sheetPr/>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -1565,349 +2349,349 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2">
+      <c r="A1" s="13"/>
+      <c r="B1" s="14">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="14">
         <v>2</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" customHeight="1" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" customHeight="1" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" ht="89" customHeight="1" spans="1:3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
     </row>
     <row r="8" customHeight="1" spans="1:8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14">
         <v>3</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="14">
         <v>4</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="14">
         <v>5</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="14">
         <v>6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="14">
         <v>7</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="14">
         <v>8</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:8">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" customHeight="1" spans="1:8">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" customHeight="1" spans="1:8">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" ht="162" customHeight="1" spans="1:8">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="17" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="15" customHeight="1" spans="1:8">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14">
+        <v>10</v>
+      </c>
+      <c r="C15" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" customHeight="1" spans="1:8">
-      <c r="A13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="15" customHeight="1" spans="1:8">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="D15" s="14">
         <v>12</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="14">
         <v>13</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="14">
         <v>14</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="14">
         <v>15</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="14">
         <v>16</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:8">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" customHeight="1" spans="1:8">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" customHeight="1" spans="1:8">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" ht="118" customHeight="1" spans="1:8">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:8">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="22" customHeight="1" spans="1:8">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14">
         <v>17</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="14">
         <v>18</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="14">
         <v>19</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="14">
         <v>20</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="14">
         <v>21</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="14">
         <v>22</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="14">
         <v>23</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:8">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" customHeight="1" spans="1:8">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" customHeight="1" spans="1:8">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" ht="119" customHeight="1" spans="1:8">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>15</v>
+      <c r="B26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:8">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="29" customHeight="1" spans="1:8">
-      <c r="A29" s="1"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="8">
         <v>24</v>
       </c>
@@ -1931,120 +2715,610 @@
       </c>
     </row>
     <row r="30" customHeight="1" spans="1:8">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
     </row>
     <row r="31" customHeight="1" spans="1:8">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" customHeight="1" spans="1:8">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33" ht="134" customHeight="1" spans="1:8">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>17</v>
+      <c r="B33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="34" customHeight="1" spans="1:8">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
-        <v>19</v>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="36" customHeight="1" spans="1:2">
-      <c r="A36" s="1"/>
+      <c r="A36" s="13"/>
       <c r="B36" s="8">
         <v>31</v>
       </c>
     </row>
     <row r="37" customHeight="1" spans="1:2">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="1"/>
+      <c r="B37" s="13"/>
     </row>
     <row r="38" customHeight="1" spans="1:2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B38" s="13"/>
     </row>
     <row r="39" customHeight="1" spans="1:2">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="13"/>
     </row>
     <row r="40" ht="87" customHeight="1" spans="1:2">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" customHeight="1" spans="1:2">
+      <c r="A41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:H41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3">
+        <v>12</v>
+      </c>
+      <c r="G8" s="3">
+        <v>13</v>
+      </c>
+      <c r="H8" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="15" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="41" customHeight="1" spans="1:2">
-      <c r="A41" s="3" t="s">
+      <c r="D15" s="3">
+        <v>17</v>
+      </c>
+      <c r="E15" s="3">
+        <v>18</v>
+      </c>
+      <c r="F15" s="3">
+        <v>19</v>
+      </c>
+      <c r="G15" s="3">
+        <v>20</v>
+      </c>
+      <c r="H15" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="22" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3">
+        <v>22</v>
+      </c>
+      <c r="C22" s="3">
+        <v>23</v>
+      </c>
+      <c r="D22" s="8">
+        <v>24</v>
+      </c>
+      <c r="E22" s="8">
+        <v>25</v>
+      </c>
+      <c r="F22" s="8">
+        <v>26</v>
+      </c>
+      <c r="G22" s="8">
+        <v>27</v>
+      </c>
+      <c r="H22" s="8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="29" s="1" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="8">
+        <v>29</v>
+      </c>
+      <c r="C29" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" ht="134" customHeight="1" spans="1:3">
+      <c r="A33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" s="1" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="36" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="10"/>
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="10"/>
+      <c r="B38" s="9"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="10"/>
+      <c r="B39" s="9"/>
+    </row>
+    <row r="40" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
+    </row>
+    <row r="41" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A41" s="10"/>
+      <c r="B41" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Tue Nov 30 09:47:41 CST 2021
</commit_message>
<xml_diff>
--- a/计划/2021学习计划.xlsx
+++ b/计划/2021学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24800" windowHeight="13180"/>
+    <workbookView windowWidth="28800" windowHeight="13180"/>
   </bookViews>
   <sheets>
     <sheet name="10" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31">
   <si>
     <t>早餐</t>
   </si>
@@ -509,6 +509,46 @@
       </rPr>
       <t>1音频</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>作业</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>作业</t>
+    </r>
   </si>
   <si>
     <r>
@@ -552,7 +592,26 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -638,7 +697,23 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">10基础知识
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -669,37 +744,6 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-10基础知识
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -711,27 +755,20 @@
         <charset val="134"/>
       </rPr>
       <t>1音频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-作业
-作业</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10基础知识
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -777,12 +814,16 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10基础知识
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -793,27 +834,62 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>作业</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+作业</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10基础知识
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -824,7 +900,17 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>20书</t>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
     </r>
     <r>
       <rPr>
@@ -841,7 +927,26 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">10基础知识
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -852,29 +957,239 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
     </r>
   </si>
   <si>
-    <t>10基础知识
-20书
+    <r>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 1音频</t>
+    </r>
   </si>
   <si>
-    <t>10基础知识
-20书
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 1音频
 作业
 作业</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+10基础知识
+20书
+1音频</t>
+    </r>
   </si>
   <si>
     <t>10基础知识
@@ -899,371 +1214,23 @@
     <t>腿</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>基础知识</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>基础知识</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t>10基础知识
+20书
 1音频</t>
-    </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>基础知识</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t>10基础知识
 20书
-10基础知识
-20书
-1音频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10基础知识</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-20书
-10基础知识
-20书
-1音频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10基础知识
-20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>基础知识</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10基础知识</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-10基础知识
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10基础知识
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-10基础知识
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
 1音频
 作业
 作业</t>
-    </r>
+  </si>
+  <si>
+    <t>问题</t>
+  </si>
+  <si>
+    <t>1. 南阳agent-4服务器内存碎片
+2. oss nginx 重复header</t>
   </si>
 </sst>
 </file>
@@ -1271,12 +1238,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1295,12 +1262,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -1313,9 +1274,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <strike/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1329,13 +1310,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -1344,9 +1318,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1354,29 +1350,6 @@
     <font>
       <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1391,6 +1364,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1399,7 +1388,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1420,61 +1424,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体-简"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <strike/>
@@ -1523,13 +1478,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1541,13 +1538,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1559,19 +1592,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1583,127 +1658,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1756,6 +1711,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1771,17 +1735,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1793,6 +1746,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1820,162 +1784,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1995,13 +1950,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2016,22 +1968,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2355,8 +2310,8 @@
   <sheetPr/>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2366,11 +2321,11 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="14">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12">
         <v>1</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="12">
         <v>2</v>
       </c>
     </row>
@@ -2378,31 +2333,31 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" customHeight="1" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" customHeight="1" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" ht="89" customHeight="1" spans="1:3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2410,30 +2365,30 @@
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
     </row>
     <row r="8" customHeight="1" spans="1:8">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12">
         <v>3</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="12">
         <v>4</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="12">
         <v>5</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="12">
         <v>6</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="12">
         <v>7</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="12">
         <v>8</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="12">
         <v>9</v>
       </c>
     </row>
@@ -2441,97 +2396,97 @@
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" customHeight="1" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" customHeight="1" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" ht="162" customHeight="1" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="H12" s="14" t="s">
         <v>11</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:8">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
     </row>
     <row r="15" customHeight="1" spans="1:8">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12">
         <v>10</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="12">
         <v>11</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="12">
         <v>12</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="12">
         <v>13</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="12">
         <v>14</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="12">
         <v>15</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="12">
         <v>16</v>
       </c>
     </row>
@@ -2539,61 +2494,61 @@
       <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" customHeight="1" spans="1:8">
       <c r="A17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" customHeight="1" spans="1:8">
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" ht="118" customHeight="1" spans="1:8">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="E19" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="F19" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2601,35 +2556,35 @@
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
     </row>
     <row r="22" customHeight="1" spans="1:8">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14">
+      <c r="A22" s="11"/>
+      <c r="B22" s="12">
         <v>17</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="12">
         <v>18</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="12">
         <v>19</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="12">
         <v>20</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="12">
         <v>21</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="12">
         <v>22</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="12">
         <v>23</v>
       </c>
     </row>
@@ -2637,97 +2592,97 @@
       <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" customHeight="1" spans="1:8">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
     </row>
     <row r="25" customHeight="1" spans="1:8">
       <c r="A25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
     </row>
     <row r="26" ht="119" customHeight="1" spans="1:8">
       <c r="A26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="16" t="s">
+      <c r="C26" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="16" t="s">
+      <c r="D26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H26" s="16" t="s">
-        <v>18</v>
+      <c r="E26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:8">
       <c r="A27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
     </row>
     <row r="29" customHeight="1" spans="1:8">
-      <c r="A29" s="13"/>
-      <c r="B29" s="8">
+      <c r="A29" s="11"/>
+      <c r="B29" s="7">
         <v>24</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="7">
         <v>25</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="7">
         <v>26</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="7">
         <v>27</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="7">
         <v>28</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="7">
         <v>29</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="7">
         <v>30</v>
       </c>
     </row>
@@ -2735,83 +2690,83 @@
       <c r="A30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
     </row>
     <row r="31" customHeight="1" spans="1:8">
       <c r="A31" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
     </row>
     <row r="32" customHeight="1" spans="1:8">
       <c r="A32" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
     </row>
     <row r="33" ht="134" customHeight="1" spans="1:8">
       <c r="A33" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>20</v>
+      <c r="B33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="34" customHeight="1" spans="1:8">
       <c r="A34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13" t="s">
-        <v>22</v>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="36" customHeight="1" spans="1:2">
-      <c r="A36" s="13"/>
-      <c r="B36" s="8">
+      <c r="A36" s="11"/>
+      <c r="B36" s="7">
         <v>31</v>
       </c>
     </row>
@@ -2819,33 +2774,33 @@
       <c r="A37" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="13"/>
+      <c r="B37" s="11"/>
     </row>
     <row r="38" customHeight="1" spans="1:2">
       <c r="A38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="13"/>
+      <c r="B38" s="11"/>
     </row>
     <row r="39" customHeight="1" spans="1:2">
       <c r="A39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="13"/>
+      <c r="B39" s="11"/>
     </row>
     <row r="40" ht="87" customHeight="1" spans="1:2">
       <c r="A40" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="16" t="s">
-        <v>19</v>
+      <c r="B40" s="17" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="41" customHeight="1" spans="1:2">
       <c r="A41" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="13"/>
+      <c r="B41" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -2856,10 +2811,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2934,82 +2889,84 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="H7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3">
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
         <v>8</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C9" s="3">
         <v>9</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="3">
         <v>10</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E9" s="3">
         <v>11</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F9" s="3">
         <v>12</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G9" s="3">
         <v>13</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H9" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
     </row>
     <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3021,7 +2978,7 @@
     </row>
     <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A11" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3031,83 +2988,83 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
         <v>17</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="15" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3">
-        <v>15</v>
-      </c>
-      <c r="C15" s="3">
-        <v>16</v>
-      </c>
-      <c r="D15" s="3">
-        <v>17</v>
-      </c>
-      <c r="E15" s="3">
+      <c r="E16" s="3">
         <v>18</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F16" s="3">
         <v>19</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G16" s="3">
         <v>20</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H16" s="3">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
     </row>
     <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A17" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -3119,7 +3076,7 @@
     </row>
     <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A18" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3129,83 +3086,83 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A20" s="4" t="s">
+      <c r="B20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="22" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
         <v>22</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D23" s="7">
         <v>24</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E23" s="7">
         <v>25</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F23" s="7">
         <v>26</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G23" s="7">
         <v>27</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H23" s="7">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A23" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
     </row>
     <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A24" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3217,7 +3174,7 @@
     </row>
     <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A25" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3227,115 +3184,127 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A27" s="4" t="s">
+      <c r="B27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="29" s="1" customFormat="1" customHeight="1" spans="1:3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="8">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="7">
         <v>29</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C30" s="7">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:3">
-      <c r="A30" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:3">
       <c r="A31" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="1:3">
       <c r="A32" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="134" customHeight="1" spans="1:3">
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:3">
       <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:3">
+      <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" s="1" customFormat="1" customHeight="1" spans="1:3">
-      <c r="A34" s="4" t="s">
+      <c r="B34" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="36" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="10"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="9"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="8"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
-    </row>
-    <row r="40" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-    </row>
-    <row r="41" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="9"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="8"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="9"/>
+      <c r="B40" s="8"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="9"/>
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="9"/>
+      <c r="B42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Wed Dec 15 22:54:33 CST 2021
</commit_message>
<xml_diff>
--- a/计划/2021学习计划.xlsx
+++ b/计划/2021学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="1"/>
+    <workbookView windowHeight="16780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="10" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
   <si>
     <t>早餐</t>
   </si>
@@ -1063,6 +1063,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">10基础知识
@@ -1094,6 +1095,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">10基础知识
@@ -1127,6 +1129,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">10基础知识
@@ -1176,6 +1179,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10基础知识
 </t>
     </r>
@@ -1274,6 +1283,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10基础知识
 20书</t>
     </r>
@@ -1281,49 +1297,184 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
     </r>
   </si>
   <si>
     <r>
-      <t>10基础知识</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10基础知识
+20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
     </r>
   </si>
   <si>
     <r>
-      <t>10基础知识
-20书</t>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <t>肩</t>
+  </si>
+  <si>
+    <t>胸</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
     </r>
     <r>
       <rPr>
@@ -1342,10 +1493,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1392,6 +1543,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -1399,8 +1558,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1408,14 +1599,6 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1431,7 +1614,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1439,24 +1622,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1484,6 +1660,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1491,46 +1681,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1564,6 +1715,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1576,7 +1733,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1594,19 +1859,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1618,151 +1907,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1791,24 +1942,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1824,6 +1957,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1835,30 +1977,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1888,153 +2006,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2054,19 +2205,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2078,22 +2232,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2428,11 +2579,11 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="14">
+      <c r="A1" s="15"/>
+      <c r="B1" s="16">
         <v>1</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="16">
         <v>2</v>
       </c>
     </row>
@@ -2440,31 +2591,31 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
     </row>
     <row r="3" customHeight="1" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" customHeight="1" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" ht="89" customHeight="1" spans="1:3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2472,30 +2623,30 @@
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
     </row>
     <row r="8" customHeight="1" spans="1:8">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16">
         <v>3</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="16">
         <v>4</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="16">
         <v>5</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="16">
         <v>6</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="16">
         <v>7</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="16">
         <v>8</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="16">
         <v>9</v>
       </c>
     </row>
@@ -2503,61 +2654,61 @@
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" customHeight="1" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" customHeight="1" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" ht="162" customHeight="1" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2565,35 +2716,35 @@
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="15" customHeight="1" spans="1:8">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16">
         <v>10</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="16">
         <v>11</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="16">
         <v>12</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="16">
         <v>13</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="16">
         <v>14</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="16">
         <v>15</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="16">
         <v>16</v>
       </c>
     </row>
@@ -2601,61 +2752,61 @@
       <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" customHeight="1" spans="1:8">
       <c r="A17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" customHeight="1" spans="1:8">
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" ht="118" customHeight="1" spans="1:8">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2663,35 +2814,35 @@
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="22" customHeight="1" spans="1:8">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16">
         <v>17</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="16">
         <v>18</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="16">
         <v>19</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="16">
         <v>20</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="16">
         <v>21</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="16">
         <v>22</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="16">
         <v>23</v>
       </c>
     </row>
@@ -2699,52 +2850,52 @@
       <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" customHeight="1" spans="1:8">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
     </row>
     <row r="25" customHeight="1" spans="1:8">
       <c r="A25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
     </row>
     <row r="26" ht="119" customHeight="1" spans="1:8">
       <c r="A26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F26" s="6" t="s">
@@ -2761,35 +2912,35 @@
       <c r="A27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="29" customHeight="1" spans="1:8">
-      <c r="A29" s="13"/>
-      <c r="B29" s="9">
+      <c r="A29" s="15"/>
+      <c r="B29" s="10">
         <v>24</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="10">
         <v>25</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="10">
         <v>26</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="10">
         <v>27</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="10">
         <v>28</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="10">
         <v>29</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="10">
         <v>30</v>
       </c>
     </row>
@@ -2797,37 +2948,37 @@
       <c r="A30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" customHeight="1" spans="1:8">
       <c r="A31" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" customHeight="1" spans="1:8">
       <c r="A32" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
     </row>
     <row r="33" ht="134" customHeight="1" spans="1:8">
       <c r="A33" s="4" t="s">
@@ -2839,19 +2990,19 @@
       <c r="C33" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G33" s="18" t="s">
+      <c r="G33" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="18" t="s">
+      <c r="H33" s="17" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2859,21 +3010,21 @@
       <c r="A34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13" t="s">
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13" t="s">
+      <c r="G34" s="15"/>
+      <c r="H34" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" customHeight="1" spans="1:2">
-      <c r="A36" s="13"/>
-      <c r="B36" s="9">
+      <c r="A36" s="15"/>
+      <c r="B36" s="10">
         <v>31</v>
       </c>
     </row>
@@ -2881,25 +3032,25 @@
       <c r="A37" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="13"/>
+      <c r="B37" s="15"/>
     </row>
     <row r="38" customHeight="1" spans="1:2">
       <c r="A38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="13"/>
+      <c r="B38" s="15"/>
     </row>
     <row r="39" customHeight="1" spans="1:2">
       <c r="A39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="13"/>
+      <c r="B39" s="15"/>
     </row>
     <row r="40" ht="87" customHeight="1" spans="1:2">
       <c r="A40" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="17" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2907,7 +3058,7 @@
       <c r="A41" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="13"/>
+      <c r="B41" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -2920,8 +3071,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3010,10 +3161,10 @@
       <c r="F5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3026,8 +3177,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3117,7 +3268,7 @@
       <c r="C13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="6" t="s">
@@ -3126,10 +3277,10 @@
       <c r="F13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3224,10 +3375,10 @@
       <c r="F20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3251,19 +3402,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="10">
         <v>24</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="10">
         <v>25</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="10">
         <v>26</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="10">
         <v>27</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="10">
         <v>28</v>
       </c>
     </row>
@@ -3322,10 +3473,10 @@
       <c r="F27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3343,13 +3494,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="9">
+      <c r="B30" s="10">
         <v>29</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="10">
         <v>30</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="10">
         <v>31</v>
       </c>
     </row>
@@ -3400,28 +3551,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="11"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="11"/>
-      <c r="B40" s="10"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="11"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="11"/>
-      <c r="B42" s="10"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3434,8 +3585,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3519,15 +3670,15 @@
         <v>30</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3540,8 +3691,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -3624,24 +3775,24 @@
         <v>3</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="D13" s="8" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3653,9 +3804,13 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A16" s="2"/>
@@ -3721,11 +3876,11 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>26</v>
+      <c r="B20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>26</v>
@@ -3736,10 +3891,10 @@
       <c r="F20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3763,19 +3918,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="10">
         <v>24</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="10">
         <v>25</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="10">
         <v>26</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="10">
         <v>27</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="10">
         <v>28</v>
       </c>
     </row>
@@ -3834,10 +3989,10 @@
       <c r="F27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3855,10 +4010,10 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:3">
       <c r="A30" s="2"/>
-      <c r="B30" s="9">
+      <c r="B30" s="10">
         <v>29</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="10">
         <v>30</v>
       </c>
     </row>
@@ -3902,28 +4057,28 @@
       <c r="C35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="11"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="11"/>
-      <c r="B40" s="10"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="11"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="11"/>
-      <c r="B42" s="10"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Sat Dec 25 21:38:36 CST 2021
</commit_message>
<xml_diff>
--- a/计划/2021学习计划.xlsx
+++ b/计划/2021学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16780" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="10" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39">
   <si>
     <t>早餐</t>
   </si>
@@ -1386,7 +1386,17 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
     </r>
   </si>
   <si>
@@ -1408,20 +1418,40 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
     </r>
   </si>
   <si>
@@ -1429,6 +1459,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">10基础知识
@@ -1439,7 +1470,7 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>20书</t>
@@ -1452,7 +1483,9 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频</t>
+1音频
+作业
+作业</t>
     </r>
   </si>
   <si>
@@ -1463,6 +1496,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10基础知识
 </t>
     </r>
@@ -1472,6 +1511,37 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t>20书</t>
@@ -1493,10 +1563,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1559,14 +1629,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1574,24 +1636,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1614,7 +1660,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1622,9 +1684,39 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1638,22 +1730,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1668,20 +1752,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1733,7 +1803,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1745,73 +1929,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1823,19 +1965,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1847,73 +1977,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1942,17 +2012,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1961,6 +2025,17 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1996,13 +2071,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2012,15 +2091,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2044,142 +2114,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2214,32 +2284,32 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2579,11 +2649,11 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="16">
+      <c r="A1" s="14"/>
+      <c r="B1" s="15">
         <v>1</v>
       </c>
-      <c r="C1" s="16">
+      <c r="C1" s="15">
         <v>2</v>
       </c>
     </row>
@@ -2591,22 +2661,22 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" customHeight="1" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
     </row>
     <row r="4" customHeight="1" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" ht="89" customHeight="1" spans="1:3">
       <c r="A5" s="4" t="s">
@@ -2623,30 +2693,30 @@
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
     </row>
     <row r="8" customHeight="1" spans="1:8">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15">
         <v>3</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="15">
         <v>4</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="15">
         <v>5</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="15">
         <v>6</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="15">
         <v>7</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="15">
         <v>8</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="15">
         <v>9</v>
       </c>
     </row>
@@ -2654,37 +2724,37 @@
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" customHeight="1" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" customHeight="1" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="12" ht="162" customHeight="1" spans="1:8">
       <c r="A12" s="4" t="s">
@@ -2716,35 +2786,35 @@
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="15" customHeight="1" spans="1:8">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15">
         <v>10</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="15">
         <v>11</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="15">
         <v>12</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="15">
         <v>13</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="15">
         <v>14</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="15">
         <v>15</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="15">
         <v>16</v>
       </c>
     </row>
@@ -2752,37 +2822,37 @@
       <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
     </row>
     <row r="17" customHeight="1" spans="1:8">
       <c r="A17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
     </row>
     <row r="18" customHeight="1" spans="1:8">
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
     </row>
     <row r="19" ht="118" customHeight="1" spans="1:8">
       <c r="A19" s="4" t="s">
@@ -2803,10 +2873,10 @@
       <c r="F19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="16" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2814,35 +2884,35 @@
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="22" customHeight="1" spans="1:8">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15">
         <v>17</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="15">
         <v>18</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="15">
         <v>19</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="15">
         <v>20</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="15">
         <v>21</v>
       </c>
-      <c r="G22" s="16">
+      <c r="G22" s="15">
         <v>22</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="15">
         <v>23</v>
       </c>
     </row>
@@ -2850,49 +2920,49 @@
       <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" customHeight="1" spans="1:8">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
     </row>
     <row r="25" customHeight="1" spans="1:8">
       <c r="A25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
     </row>
     <row r="26" ht="119" customHeight="1" spans="1:8">
       <c r="A26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="16" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="18" t="s">
@@ -2912,35 +2982,35 @@
       <c r="A27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="29" customHeight="1" spans="1:8">
-      <c r="A29" s="15"/>
-      <c r="B29" s="10">
+      <c r="A29" s="14"/>
+      <c r="B29" s="9">
         <v>24</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="9">
         <v>25</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="9">
         <v>26</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="9">
         <v>27</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29" s="9">
         <v>28</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="9">
         <v>29</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29" s="9">
         <v>30</v>
       </c>
     </row>
@@ -2948,37 +3018,37 @@
       <c r="A30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" customHeight="1" spans="1:8">
       <c r="A31" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
     </row>
     <row r="32" customHeight="1" spans="1:8">
       <c r="A32" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
     </row>
     <row r="33" ht="134" customHeight="1" spans="1:8">
       <c r="A33" s="4" t="s">
@@ -3010,21 +3080,21 @@
       <c r="A34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15" t="s">
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15" t="s">
+      <c r="G34" s="14"/>
+      <c r="H34" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" customHeight="1" spans="1:2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="10">
+      <c r="A36" s="14"/>
+      <c r="B36" s="9">
         <v>31</v>
       </c>
     </row>
@@ -3032,19 +3102,19 @@
       <c r="A37" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="15"/>
+      <c r="B37" s="14"/>
     </row>
     <row r="38" customHeight="1" spans="1:2">
       <c r="A38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="15"/>
+      <c r="B38" s="14"/>
     </row>
     <row r="39" customHeight="1" spans="1:2">
       <c r="A39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="15"/>
+      <c r="B39" s="14"/>
     </row>
     <row r="40" ht="87" customHeight="1" spans="1:2">
       <c r="A40" s="4" t="s">
@@ -3058,7 +3128,7 @@
       <c r="A41" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="15"/>
+      <c r="B41" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3161,10 +3231,10 @@
       <c r="F5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3177,8 +3247,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9" t="s">
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3268,7 +3338,7 @@
       <c r="C13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="6" t="s">
@@ -3277,10 +3347,10 @@
       <c r="F13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3375,10 +3445,10 @@
       <c r="F20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3402,19 +3472,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>24</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="9">
         <v>25</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="9">
         <v>26</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="9">
         <v>27</v>
       </c>
-      <c r="H23" s="10">
+      <c r="H23" s="9">
         <v>28</v>
       </c>
     </row>
@@ -3473,10 +3543,10 @@
       <c r="F27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3494,13 +3564,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <v>29</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="9">
         <v>30</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="9">
         <v>31</v>
       </c>
     </row>
@@ -3551,28 +3621,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="11"/>
-      <c r="B37" s="12"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="12"/>
-      <c r="B38" s="11"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="10"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="12"/>
-      <c r="B39" s="11"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="12"/>
-      <c r="B40" s="11"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="10"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="12"/>
-      <c r="B41" s="13"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="12"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="12"/>
-      <c r="B42" s="11"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3585,8 +3655,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3672,13 +3742,13 @@
       <c r="E5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3691,8 +3761,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -3777,23 +3847,23 @@
       <c r="B13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="G13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="H13" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3876,25 +3946,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3918,19 +3988,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>24</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="9">
         <v>25</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="9">
         <v>26</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="9">
         <v>27</v>
       </c>
-      <c r="H23" s="10">
+      <c r="H23" s="9">
         <v>28</v>
       </c>
     </row>
@@ -3989,10 +4059,10 @@
       <c r="F27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4010,10 +4080,10 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:3">
       <c r="A30" s="2"/>
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <v>29</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="9">
         <v>30</v>
       </c>
     </row>
@@ -4057,28 +4127,28 @@
       <c r="C35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="11"/>
-      <c r="B37" s="12"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="12"/>
-      <c r="B38" s="11"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="10"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="12"/>
-      <c r="B39" s="11"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="12"/>
-      <c r="B40" s="11"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="10"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="12"/>
-      <c r="B41" s="13"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="12"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="12"/>
-      <c r="B42" s="11"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Sat Dec 25 21:40:29 CST 2021
</commit_message>
<xml_diff>
--- a/计划/2021学习计划.xlsx
+++ b/计划/2021学习计划.xlsx
@@ -3655,8 +3655,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
Wed Dec 29 06:34:12 CST 2021
</commit_message>
<xml_diff>
--- a/计划/2021学习计划.xlsx
+++ b/计划/2021学习计划.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
   <si>
     <t>早餐</t>
   </si>
@@ -1314,6 +1314,33 @@
     </r>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
+    </r>
+  </si>
+  <si>
     <t>10基础知识
 20书
 1音频/视频
@@ -1406,7 +1433,16 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">10基础知识
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -1472,7 +1508,16 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">10基础知识
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -1525,7 +1570,16 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">10基础知识
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -1546,7 +1600,17 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频</t>
     </r>
   </si>
   <si>
@@ -1579,6 +1643,31 @@
       </rPr>
       <t xml:space="preserve">
 1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
     </r>
   </si>
   <si>
@@ -2331,14 +2420,14 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2678,11 +2767,11 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:3">
-      <c r="A1" s="14"/>
-      <c r="B1" s="15">
+      <c r="A1" s="15"/>
+      <c r="B1" s="16">
         <v>1</v>
       </c>
-      <c r="C1" s="15">
+      <c r="C1" s="16">
         <v>2</v>
       </c>
     </row>
@@ -2690,22 +2779,22 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
     </row>
     <row r="3" customHeight="1" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" customHeight="1" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" ht="89" customHeight="1" spans="1:3">
       <c r="A5" s="4" t="s">
@@ -2722,30 +2811,30 @@
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
     </row>
     <row r="8" customHeight="1" spans="1:8">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16">
         <v>3</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="16">
         <v>4</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="16">
         <v>5</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="16">
         <v>6</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="16">
         <v>7</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="16">
         <v>8</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="16">
         <v>9</v>
       </c>
     </row>
@@ -2753,37 +2842,37 @@
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" customHeight="1" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" customHeight="1" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" ht="162" customHeight="1" spans="1:8">
       <c r="A12" s="4" t="s">
@@ -2815,35 +2904,35 @@
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="15" customHeight="1" spans="1:8">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16">
         <v>10</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="16">
         <v>11</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="16">
         <v>12</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="16">
         <v>13</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="16">
         <v>14</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="16">
         <v>15</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="16">
         <v>16</v>
       </c>
     </row>
@@ -2851,37 +2940,37 @@
       <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" customHeight="1" spans="1:8">
       <c r="A17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" customHeight="1" spans="1:8">
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" ht="118" customHeight="1" spans="1:8">
       <c r="A19" s="4" t="s">
@@ -2902,10 +2991,10 @@
       <c r="F19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="14" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2913,35 +3002,35 @@
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="22" customHeight="1" spans="1:8">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16">
         <v>17</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="16">
         <v>18</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="16">
         <v>19</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="16">
         <v>20</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="16">
         <v>21</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="16">
         <v>22</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="16">
         <v>23</v>
       </c>
     </row>
@@ -2949,37 +3038,37 @@
       <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" customHeight="1" spans="1:8">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
     </row>
     <row r="25" customHeight="1" spans="1:8">
       <c r="A25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
     </row>
     <row r="26" ht="119" customHeight="1" spans="1:8">
       <c r="A26" s="4" t="s">
@@ -2988,10 +3077,10 @@
       <c r="B26" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="18" t="s">
@@ -3011,16 +3100,16 @@
       <c r="A27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="29" customHeight="1" spans="1:8">
-      <c r="A29" s="14"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="9">
         <v>24</v>
       </c>
@@ -3047,37 +3136,37 @@
       <c r="A30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" customHeight="1" spans="1:8">
       <c r="A31" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" customHeight="1" spans="1:8">
       <c r="A32" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
     </row>
     <row r="33" ht="134" customHeight="1" spans="1:8">
       <c r="A33" s="4" t="s">
@@ -3109,20 +3198,20 @@
       <c r="A34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14" t="s">
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14" t="s">
+      <c r="G34" s="15"/>
+      <c r="H34" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" customHeight="1" spans="1:2">
-      <c r="A36" s="14"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="9">
         <v>31</v>
       </c>
@@ -3131,19 +3220,19 @@
       <c r="A37" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="14"/>
+      <c r="B37" s="15"/>
     </row>
     <row r="38" customHeight="1" spans="1:2">
       <c r="A38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="14"/>
+      <c r="B38" s="15"/>
     </row>
     <row r="39" customHeight="1" spans="1:2">
       <c r="A39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="14"/>
+      <c r="B39" s="15"/>
     </row>
     <row r="40" ht="87" customHeight="1" spans="1:2">
       <c r="A40" s="4" t="s">
@@ -3157,7 +3246,7 @@
       <c r="A41" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="14"/>
+      <c r="B41" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3684,8 +3773,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3778,7 +3867,7 @@
         <v>31</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -3874,13 +3963,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>12</v>
@@ -3888,11 +3977,11 @@
       <c r="F13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="8" t="s">
+      <c r="G13" s="14" t="s">
         <v>35</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3904,11 +3993,11 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3975,11 +4064,11 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>38</v>
+      <c r="B20" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>18</v>
@@ -3988,13 +4077,13 @@
         <v>18</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4074,25 +4163,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4100,10 +4189,14 @@
         <v>6</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
@@ -4142,10 +4235,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:3">

</xml_diff>

<commit_message>
Fri Jan  7 04:25:37 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2021学习计划.xlsx
+++ b/计划/2021学习计划.xlsx
@@ -3467,8 +3467,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3763,7 +3763,7 @@
         <v>30</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Wed Jan 12 02:23:01 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2021学习计划.xlsx
+++ b/计划/2021学习计划.xlsx
@@ -1389,13 +1389,16 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10基础知识
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -2601,10 +2604,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2937,7 +2940,7 @@
   <sheetPr/>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -3172,10 +3175,10 @@
       <c r="F19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H19" s="14" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3258,10 +3261,10 @@
       <c r="B26" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="9" t="s">
@@ -3440,8 +3443,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3530,10 +3533,10 @@
       <c r="F5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3546,8 +3549,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15" t="s">
+      <c r="G6" s="15"/>
+      <c r="H6" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3637,7 +3640,7 @@
       <c r="C13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="15" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="6" t="s">
@@ -3646,10 +3649,10 @@
       <c r="F13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3739,15 +3742,15 @@
         <v>31</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3842,10 +3845,10 @@
       <c r="F27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3954,8 +3957,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4047,7 +4050,7 @@
       <c r="G5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="15" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4060,8 +4063,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -4158,10 +4161,10 @@
       <c r="F13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4254,16 +4257,16 @@
       <c r="D20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="15" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4358,10 +4361,10 @@
       <c r="F27" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="15" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fri Jan 14 02:59:57 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2021学习计划.xlsx
+++ b/计划/2021学习计划.xlsx
@@ -11,12 +11,12 @@
     <sheet name="11" sheetId="2" r:id="rId2"/>
     <sheet name="12" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46">
   <si>
     <t>早餐</t>
   </si>
@@ -1352,6 +1352,33 @@
       </rPr>
       <t xml:space="preserve">
 1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频
+作业</t>
     </r>
   </si>
   <si>
@@ -3443,8 +3470,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3644,7 +3671,7 @@
         <v>26</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>26</v>
@@ -3745,13 +3772,13 @@
         <v>27</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3957,7 +3984,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -4033,25 +4060,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -4147,13 +4174,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>12</v>
@@ -4162,10 +4189,10 @@
         <v>12</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4177,11 +4204,11 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4249,25 +4276,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4347,25 +4374,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4379,7 +4406,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -4425,13 +4452,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">

</xml_diff>

<commit_message>
Fri Jan 21 04:16:40 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2021学习计划.xlsx
+++ b/计划/2021学习计划.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="10" sheetId="1" r:id="rId1"/>
     <sheet name="11" sheetId="2" r:id="rId2"/>
     <sheet name="12" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50">
   <si>
     <t>早餐</t>
   </si>
@@ -1269,6 +1269,53 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10基础知识
 </t>
     </r>
@@ -1286,6 +1333,110 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频
+作业</t>
+    </r>
+  </si>
+  <si>
+    <t>问题</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1. 南阳agent-4服务器内存碎片</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+2. oss nginx 重复header</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -1299,63 +1450,13 @@
 作业</t>
   </si>
   <si>
-    <t>问题</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1. 南阳agent-4服务器内存碎片</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-2. oss nginx 重复header</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10基础知识
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
-    </r>
-  </si>
-  <si>
-    <r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10基础知识
 </t>
     </r>
@@ -1416,6 +1517,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>10基础知识</t>
     </r>
     <r>
@@ -1815,6 +1923,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>10基础知识</t>
     </r>
     <r>
@@ -1896,6 +2011,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">10基础知识
@@ -1928,10 +2044,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1987,7 +2103,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1995,6 +2111,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2016,11 +2139,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2032,22 +2169,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2071,7 +2194,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2079,7 +2210,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2093,32 +2224,17 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2168,79 +2284,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2252,91 +2296,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2349,6 +2309,162 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2378,21 +2494,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -2410,17 +2511,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2451,15 +2558,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2474,147 +2572,165 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3003,7 +3119,7 @@
   <sheetPr/>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -3506,8 +3622,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3581,31 +3697,31 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -3614,7 +3730,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="15"/>
       <c r="H6" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3698,25 +3814,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3796,25 +3912,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3894,10 +4010,10 @@
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>26</v>
@@ -3909,10 +4025,10 @@
         <v>26</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4020,8 +4136,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4096,30 +4212,30 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -4210,13 +4326,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>12</v>
@@ -4225,10 +4341,10 @@
         <v>12</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4240,11 +4356,11 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4312,25 +4428,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4410,25 +4526,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4442,7 +4558,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -4488,13 +4604,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">

</xml_diff>

<commit_message>
Fri Jan 28 00:01:40 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2021学习计划.xlsx
+++ b/计划/2021学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="1"/>
+    <workbookView windowHeight="13180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="10" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
   <si>
     <t>早餐</t>
   </si>
@@ -1270,78 +1270,11 @@
   <si>
     <r>
       <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10基础知识</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10基础知识
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
-    </r>
-  </si>
-  <si>
-    <r>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10基础知识
 </t>
     </r>
@@ -1394,6 +1327,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10基础知识
 </t>
     </r>
@@ -1411,6 +1349,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -1419,6 +1358,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10基础知识
 </t>
     </r>
@@ -1437,6 +1382,58 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频
+作业</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -1448,39 +1445,6 @@
 20书
 1音频
 作业</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10基础知识
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频
-作业</t>
-    </r>
   </si>
   <si>
     <r>
@@ -2044,10 +2008,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -2094,14 +2058,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -2109,17 +2065,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2131,16 +2081,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2155,7 +2113,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2169,11 +2142,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2201,21 +2180,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -2224,7 +2188,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2232,7 +2196,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2284,7 +2248,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2296,7 +2416,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2308,163 +2428,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2493,6 +2457,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2511,8 +2493,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2572,171 +2554,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3622,8 +3586,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3698,30 +3662,30 @@
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>29</v>
-      </c>
       <c r="H5" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -3730,7 +3694,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="15"/>
       <c r="H6" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3814,25 +3778,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="H13" s="15" t="s">
         <v>32</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3921,16 +3885,16 @@
         <v>18</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4010,19 +3974,19 @@
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="G27" s="15" t="s">
         <v>34</v>
@@ -4212,30 +4176,30 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="15" t="s">
         <v>37</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -4326,13 +4290,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="D13" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>12</v>
@@ -4341,10 +4305,10 @@
         <v>12</v>
       </c>
       <c r="G13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4356,11 +4320,11 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4428,25 +4392,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="G20" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="H20" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4526,25 +4490,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="D27" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4558,7 +4522,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -4604,13 +4568,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">

</xml_diff>

<commit_message>
Fri Feb  4 04:59:37 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2021学习计划.xlsx
+++ b/计划/2021学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20380" windowHeight="16760"/>
+    <workbookView windowHeight="16780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="10" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
   <si>
     <t>早餐</t>
   </si>
@@ -1087,38 +1087,6 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10基础知识
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
 1音频
 作业
 作业</t>
@@ -1179,12 +1147,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">10基础知识
 </t>
     </r>
@@ -1242,6 +1204,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10基础知识
 </t>
     </r>
@@ -1259,6 +1226,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -1279,6 +1247,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -1287,6 +1256,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10基础知识
 </t>
     </r>
@@ -1304,29 +1278,35 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
 10基础知识
-20书
-1音频</t>
-    </r>
-  </si>
-  <si>
-    <t>10基础知识
-20书
-10基础知识
-20书
-1音频</t>
-  </si>
-  <si>
-    <t>10基础知识
-20书
-10基础知识
-20书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 1音频
 作业
 作业</t>
+    </r>
   </si>
   <si>
     <t>背</t>
@@ -1335,12 +1315,44 @@
     <t>腿</t>
   </si>
   <si>
-    <t>10基础知识
-20书
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 1音频</t>
+    </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10基础知识
 </t>
     </r>
@@ -1363,6 +1375,38 @@
         <charset val="134"/>
       </rPr>
       <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10基础知识
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20书</t>
     </r>
     <r>
       <rPr>
@@ -1438,6 +1482,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">10基础知识
@@ -1448,7 +1493,7 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>20书</t>
@@ -1458,135 +1503,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10基础知识
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">10基础知识
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频
-作业</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10基础知识</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">10基础知识
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2119,6 +2035,51 @@
   </si>
   <si>
     <r>
+      <t>10基础知识</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
@@ -2156,9 +2117,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -2205,18 +2166,11 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2228,8 +2182,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2251,31 +2228,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2289,23 +2243,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2321,29 +2283,28 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2395,54 +2356,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2455,7 +2368,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2467,19 +2494,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2491,91 +2536,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2604,11 +2565,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2617,7 +2584,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2637,15 +2604,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2657,6 +2615,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2678,26 +2647,18 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2706,152 +2667,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2882,6 +2843,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2894,9 +2858,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2905,9 +2866,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -3230,8 +3188,8 @@
   <sheetPr/>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3465,10 +3423,10 @@
       <c r="F19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3548,26 +3506,26 @@
       <c r="A26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="H26" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:8">
@@ -3647,25 +3605,25 @@
         <v>3</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="E33" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G33" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H33" s="18" t="s">
-        <v>25</v>
+      <c r="H33" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="34" customHeight="1" spans="1:8">
@@ -3677,11 +3635,11 @@
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
       <c r="F34" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G34" s="16"/>
       <c r="H34" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" customHeight="1" spans="1:2">
@@ -3712,8 +3670,8 @@
       <c r="A40" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>28</v>
+      <c r="B40" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="41" customHeight="1" spans="1:2">
@@ -3733,7 +3691,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -3812,27 +3770,27 @@
         <v>17</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -3840,8 +3798,8 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="15"/>
-      <c r="H6" s="14" t="s">
-        <v>32</v>
+      <c r="H6" s="10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3854,10 +3812,10 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3925,25 +3883,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4023,25 +3981,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4121,25 +4079,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4195,13 +4153,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4213,28 +4171,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="11"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="11"/>
-      <c r="B40" s="10"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="11"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="11"/>
-      <c r="B42" s="10"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4247,8 +4205,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4323,30 +4281,30 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="14" t="s">
-        <v>39</v>
+      <c r="G5" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -4366,10 +4324,10 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4437,13 +4395,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>12</v>
@@ -4451,11 +4409,11 @@
       <c r="F13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>44</v>
+      <c r="G13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4467,11 +4425,11 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4539,25 +4497,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>49</v>
+      <c r="E20" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4637,25 +4595,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4664,12 +4622,12 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -4715,13 +4673,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4733,28 +4691,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="11"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="11"/>
-      <c r="B40" s="10"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="11"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="11"/>
-      <c r="B42" s="10"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>